<commit_message>
Corrección pruebas 2 listas
</commit_message>
<xml_diff>
--- a/clases/clase_12/notas_prueba2.xlsx
+++ b/clases/clase_12/notas_prueba2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fran/Desktop/Ayudantías Cuanti R/mc2/clases/clase_12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A9DD82-F762-1D4D-8891-471560F2A711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0FF7BB-4E41-8B4A-B2C9-F46FB2EA1AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" xr2:uid="{4B4FE8C0-9535-43E1-81A6-0C70ED611A4C}"/>
   </bookViews>
@@ -866,8 +866,8 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
+      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2678,14 +2678,51 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="2"/>
-      <c r="T37" s="3"/>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L37" s="3">
+        <v>2</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="O37" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="P37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37" s="2">
+        <v>0.5</v>
+      </c>
       <c r="U37" s="2"/>
       <c r="W37" s="3"/>
       <c r="X37" s="2"/>
@@ -2694,28 +2731,56 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5">
+        <v>2</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2</v>
+      </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="6"/>
+      <c r="J38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K38" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L38" s="3">
+        <v>2</v>
+      </c>
+      <c r="M38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="O38" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="P38" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>2</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38" s="2">
+        <v>0.5</v>
+      </c>
       <c r="U38" s="4"/>
       <c r="V38" s="5"/>
       <c r="W38" s="6"/>

</xml_diff>